<commit_message>
add line chart test case
</commit_message>
<xml_diff>
--- a/zss-ngmodel/src/test/java/org/zkoss/zss/ngmodel/book/chart.xlsx
+++ b/zss-ngmodel/src/test/java/org/zkoss/zss/ngmodel/book/chart.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="345" windowWidth="17955" windowHeight="7455" activeTab="4"/>
+    <workbookView xWindow="600" yWindow="345" windowWidth="17955" windowHeight="7455" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Area" sheetId="3" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="43">
   <si>
     <t>Internet Explorer</t>
   </si>
@@ -100,9 +100,6 @@
   </si>
   <si>
     <t>Safari</t>
-  </si>
-  <si>
-    <t>s</t>
   </si>
   <si>
     <t>A</t>
@@ -593,24 +590,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="95903744"/>
-        <c:axId val="96413568"/>
+        <c:axId val="86577920"/>
+        <c:axId val="86579456"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="95903744"/>
+        <c:axId val="86577920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="96413568"/>
+        <c:crossAx val="86579456"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="96413568"/>
+        <c:axId val="86579456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -618,7 +615,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="95903744"/>
+        <c:crossAx val="86577920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -630,7 +627,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000133" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000133" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -661,6 +658,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
     </c:title>
     <c:view3D>
       <c:perspective val="30"/>
@@ -909,26 +907,26 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="57910400"/>
-        <c:axId val="57911936"/>
-        <c:axId val="96553600"/>
+        <c:axId val="57800960"/>
+        <c:axId val="57905152"/>
+        <c:axId val="102830080"/>
       </c:line3DChart>
       <c:catAx>
-        <c:axId val="57910400"/>
+        <c:axId val="57800960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="57911936"/>
+        <c:crossAx val="57905152"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="57911936"/>
+        <c:axId val="57905152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -942,30 +940,31 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="57910400"/>
+        <c:crossAx val="57800960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:serAx>
-        <c:axId val="96553600"/>
+        <c:axId val="102830080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="1"/>
         <c:axPos val="b"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="57911936"/>
+        <c:crossAx val="57905152"/>
         <c:crosses val="autoZero"/>
       </c:serAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1041,12 +1040,13 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1125,12 +1125,13 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1399,22 +1400,22 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="69879680"/>
-        <c:axId val="69881216"/>
+        <c:axId val="69868544"/>
+        <c:axId val="69886720"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="69879680"/>
+        <c:axId val="69868544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="69881216"/>
+        <c:crossAx val="69886720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="69881216"/>
+        <c:axId val="69886720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1422,7 +1423,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="69879680"/>
+        <c:crossAx val="69868544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1434,7 +1435,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1758,24 +1759,24 @@
           <c:upBars/>
           <c:downBars/>
         </c:upDownBars>
-        <c:axId val="70043904"/>
-        <c:axId val="71442432"/>
+        <c:axId val="71454080"/>
+        <c:axId val="71480448"/>
       </c:stockChart>
       <c:catAx>
-        <c:axId val="70043904"/>
+        <c:axId val="71454080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="71442432"/>
+        <c:crossAx val="71480448"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="71442432"/>
+        <c:axId val="71480448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1783,20 +1784,19 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="70043904"/>
+        <c:crossAx val="71454080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2054,26 +2054,26 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="103245312"/>
-        <c:axId val="103246848"/>
-        <c:axId val="86618112"/>
+        <c:axId val="87190912"/>
+        <c:axId val="95895936"/>
+        <c:axId val="88073984"/>
       </c:area3DChart>
       <c:catAx>
-        <c:axId val="103245312"/>
+        <c:axId val="87190912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103246848"/>
+        <c:crossAx val="95895936"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="103246848"/>
+        <c:axId val="95895936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2082,19 +2082,19 @@
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103245312"/>
+        <c:crossAx val="87190912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:serAx>
-        <c:axId val="86618112"/>
+        <c:axId val="88073984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="1"/>
         <c:axPos val="b"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="103246848"/>
+        <c:crossAx val="95895936"/>
         <c:crosses val="autoZero"/>
       </c:serAx>
     </c:plotArea>
@@ -2105,7 +2105,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000133" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000133" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000155" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000155" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2287,11 +2287,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="104699392"/>
-        <c:axId val="104715776"/>
+        <c:axId val="96547584"/>
+        <c:axId val="96549504"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="104699392"/>
+        <c:axId val="96547584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2314,14 +2314,14 @@
           </c:tx>
         </c:title>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="104715776"/>
+        <c:crossAx val="96549504"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="104715776"/>
+        <c:axId val="96549504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2346,7 +2346,7 @@
         </c:title>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="104699392"/>
+        <c:crossAx val="96547584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2358,7 +2358,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000144" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000144" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000167" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000167" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup orientation="portrait"/>
   </c:printSettings>
 </c:chartSpace>
@@ -2594,25 +2594,25 @@
           </c:val>
         </c:ser>
         <c:shape val="box"/>
-        <c:axId val="116255744"/>
-        <c:axId val="117654272"/>
+        <c:axId val="104670336"/>
+        <c:axId val="104697856"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="116255744"/>
+        <c:axId val="104670336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="117654272"/>
+        <c:crossAx val="104697856"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="117654272"/>
+        <c:axId val="104697856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2620,7 +2620,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="116255744"/>
+        <c:crossAx val="104670336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2632,7 +2632,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000167" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000167" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000189" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000189" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup orientation="portrait"/>
   </c:printSettings>
 </c:chartSpace>
@@ -2642,9 +2642,7 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
-    <c:title>
-      <c:layout/>
-    </c:title>
+    <c:title/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
@@ -2822,25 +2820,25 @@
           <c:showVal val="1"/>
         </c:dLbls>
         <c:overlap val="-25"/>
-        <c:axId val="128554112"/>
-        <c:axId val="128555648"/>
+        <c:axId val="116201728"/>
+        <c:axId val="116253440"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="128554112"/>
+        <c:axId val="116201728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="128555648"/>
+        <c:crossAx val="116253440"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="128555648"/>
+        <c:axId val="116253440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2848,20 +2846,19 @@
         <c:axPos val="l"/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="128554112"/>
+        <c:crossAx val="116201728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000133" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000133" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000155" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000155" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3048,25 +3045,25 @@
           </c:val>
         </c:ser>
         <c:shape val="box"/>
-        <c:axId val="134008832"/>
-        <c:axId val="134010368"/>
+        <c:axId val="117763456"/>
+        <c:axId val="128525440"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="134008832"/>
+        <c:axId val="117763456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="134010368"/>
+        <c:crossAx val="128525440"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="134010368"/>
+        <c:axId val="128525440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3074,20 +3071,19 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="134008832"/>
+        <c:crossAx val="117763456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000133" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000133" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000155" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000155" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3384,7 +3380,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3395,6 +3391,21 @@
   <c:lang val="en-US"/>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Sales</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
     </c:title>
     <c:plotArea>
@@ -3488,23 +3499,23 @@
           </c:bubbleSize>
         </c:ser>
         <c:bubbleScale val="100"/>
-        <c:axId val="57740288"/>
-        <c:axId val="57750272"/>
+        <c:axId val="57336192"/>
+        <c:axId val="57337728"/>
       </c:bubbleChart>
       <c:valAx>
-        <c:axId val="57740288"/>
+        <c:axId val="57336192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="57750272"/>
+        <c:crossAx val="57337728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="57750272"/>
+        <c:axId val="57337728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3512,7 +3523,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="57740288"/>
+        <c:crossAx val="57336192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3525,7 +3536,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3789,24 +3800,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="57784576"/>
-        <c:axId val="57798656"/>
+        <c:axId val="57752960"/>
+        <c:axId val="57762944"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="57784576"/>
+        <c:axId val="57752960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="57798656"/>
+        <c:crossAx val="57762944"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="57798656"/>
+        <c:axId val="57762944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3814,19 +3825,20 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="57784576"/>
+        <c:crossAx val="57752960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4892,8 +4904,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O4" sqref="O4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4991,9 +5003,9 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
@@ -5002,12 +5014,12 @@
     <col min="1" max="1" width="25.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:2">
       <c r="A1" s="6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -5015,7 +5027,7 @@
         <v>44.6</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -5023,7 +5035,7 @@
         <v>22.08</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -5031,7 +5043,7 @@
         <v>18.170000000000002</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>23</v>
       </c>
@@ -5039,7 +5051,7 @@
         <v>9.07</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>24</v>
       </c>
@@ -5047,17 +5059,12 @@
         <v>3.38</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
         <v>25</v>
       </c>
       <c r="B7">
         <v>3.24</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="C14" t="s">
-        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -5093,45 +5100,45 @@
   <sheetData>
     <row r="1" spans="1:6" ht="17.25" thickBot="1">
       <c r="A1" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B1" s="8"/>
       <c r="C1" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="E1" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="E1" s="8" t="s">
-        <v>31</v>
-      </c>
       <c r="F1" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="17.25" thickBot="1">
       <c r="A2" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="F2" s="9" t="s">
         <v>32</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="17.25" thickBot="1">
       <c r="A3" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B3" s="10">
         <v>27.2</v>
@@ -5151,7 +5158,7 @@
     </row>
     <row r="4" spans="1:6" ht="17.25" thickBot="1">
       <c r="A4" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B4" s="9">
         <v>25.03</v>
@@ -5171,7 +5178,7 @@
     </row>
     <row r="5" spans="1:6" ht="17.25" thickBot="1">
       <c r="A5" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B5" s="10">
         <v>19.05</v>
@@ -5191,7 +5198,7 @@
     </row>
     <row r="6" spans="1:6" ht="17.25" thickBot="1">
       <c r="A6" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B6" s="9">
         <v>20.329999999999998</v>
@@ -5211,7 +5218,7 @@
     </row>
     <row r="7" spans="1:6" ht="17.25" thickBot="1">
       <c r="A7" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B7" s="10">
         <v>18.559999999999999</v>
@@ -5231,7 +5238,7 @@
     </row>
     <row r="8" spans="1:6" ht="17.25" thickBot="1">
       <c r="A8" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B8" s="10">
         <v>18.559999999999999</v>

</xml_diff>

<commit_message>
fix column width and row height. (dx1 = x offset, dy1 = y offset)
</commit_message>
<xml_diff>
--- a/zss-ngmodel/src/test/java/org/zkoss/zss/ngmodel/book/chart.xlsx
+++ b/zss-ngmodel/src/test/java/org/zkoss/zss/ngmodel/book/chart.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="345" windowWidth="17955" windowHeight="7455" activeTab="4"/>
+    <workbookView xWindow="600" yWindow="345" windowWidth="17955" windowHeight="7455"/>
   </bookViews>
   <sheets>
     <sheet name="Area" sheetId="3" r:id="rId1"/>
@@ -590,24 +590,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="72660864"/>
-        <c:axId val="73105408"/>
+        <c:axId val="70504832"/>
+        <c:axId val="70506752"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="72660864"/>
+        <c:axId val="70504832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="73105408"/>
+        <c:crossAx val="70506752"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="73105408"/>
+        <c:axId val="70506752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -615,19 +615,20 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="72660864"/>
+        <c:crossAx val="70504832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000167" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000167" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000244" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000244" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -906,26 +907,26 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="72531968"/>
-        <c:axId val="72533504"/>
-        <c:axId val="72523776"/>
+        <c:axId val="64761856"/>
+        <c:axId val="64763392"/>
+        <c:axId val="75238912"/>
       </c:line3DChart>
       <c:catAx>
-        <c:axId val="72531968"/>
+        <c:axId val="64761856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="72533504"/>
+        <c:crossAx val="64763392"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="72533504"/>
+        <c:axId val="64763392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -939,19 +940,19 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="72531968"/>
+        <c:crossAx val="64761856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:serAx>
-        <c:axId val="72523776"/>
+        <c:axId val="75238912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="1"/>
         <c:axPos val="b"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="72533504"/>
+        <c:crossAx val="64763392"/>
         <c:crosses val="autoZero"/>
       </c:serAx>
     </c:plotArea>
@@ -962,7 +963,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000133" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000133" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000211" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000211" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1043,7 +1044,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000167" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000167" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1127,7 +1128,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000189" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000189" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1396,22 +1397,22 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="73089792"/>
-        <c:axId val="73091328"/>
+        <c:axId val="67547904"/>
+        <c:axId val="67549440"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="73089792"/>
+        <c:axId val="67547904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="73091328"/>
+        <c:crossAx val="67549440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="73091328"/>
+        <c:axId val="67549440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1419,7 +1420,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="73089792"/>
+        <c:crossAx val="67547904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1431,7 +1432,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000189" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000189" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1755,24 +1756,24 @@
           <c:upBars/>
           <c:downBars/>
         </c:upDownBars>
-        <c:axId val="73135232"/>
-        <c:axId val="73136768"/>
+        <c:axId val="69940352"/>
+        <c:axId val="69941888"/>
       </c:stockChart>
       <c:catAx>
-        <c:axId val="73135232"/>
+        <c:axId val="69940352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="73136768"/>
+        <c:crossAx val="69941888"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="73136768"/>
+        <c:axId val="69941888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1780,7 +1781,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="73135232"/>
+        <c:crossAx val="69940352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1792,7 +1793,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000155" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000155" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1802,7 +1803,9 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
-    <c:title/>
+    <c:title>
+      <c:layout/>
+    </c:title>
     <c:view3D>
       <c:perspective val="30"/>
     </c:view3D>
@@ -2050,26 +2053,26 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="73190784"/>
-        <c:axId val="74678656"/>
-        <c:axId val="60181120"/>
+        <c:axId val="72437760"/>
+        <c:axId val="72439296"/>
+        <c:axId val="70380160"/>
       </c:area3DChart>
       <c:catAx>
-        <c:axId val="73190784"/>
+        <c:axId val="72437760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="74678656"/>
+        <c:crossAx val="72439296"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="74678656"/>
+        <c:axId val="72439296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2078,30 +2081,31 @@
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="73190784"/>
+        <c:crossAx val="72437760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:serAx>
-        <c:axId val="60181120"/>
+        <c:axId val="70380160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="1"/>
         <c:axPos val="b"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="74678656"/>
+        <c:crossAx val="72439296"/>
         <c:crosses val="autoZero"/>
       </c:serAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000189" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000189" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000266" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000266" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2127,6 +2131,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -2283,11 +2288,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="74881664"/>
-        <c:axId val="75041408"/>
+        <c:axId val="88132608"/>
+        <c:axId val="64222336"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="74881664"/>
+        <c:axId val="88132608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2308,16 +2313,17 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="75041408"/>
+        <c:crossAx val="64222336"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="75041408"/>
+        <c:axId val="64222336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2339,22 +2345,24 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="74881664"/>
+        <c:crossAx val="88132608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000002" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000002" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000278" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000278" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup orientation="portrait"/>
   </c:printSettings>
 </c:chartSpace>
@@ -2380,6 +2388,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
     </c:title>
     <c:view3D>
       <c:perspective val="30"/>
@@ -2590,25 +2599,25 @@
           </c:val>
         </c:ser>
         <c:shape val="box"/>
-        <c:axId val="105740928"/>
-        <c:axId val="107479808"/>
+        <c:axId val="64307200"/>
+        <c:axId val="64308736"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="105740928"/>
+        <c:axId val="64307200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="107479808"/>
+        <c:crossAx val="64308736"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="107479808"/>
+        <c:axId val="64308736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2616,19 +2625,20 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="105740928"/>
+        <c:crossAx val="64307200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000222" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000222" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000003" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000003" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup orientation="portrait"/>
   </c:printSettings>
 </c:chartSpace>
@@ -2816,25 +2826,25 @@
           <c:showVal val="1"/>
         </c:dLbls>
         <c:overlap val="-25"/>
-        <c:axId val="60338560"/>
-        <c:axId val="60340096"/>
+        <c:axId val="64360832"/>
+        <c:axId val="64362368"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="60338560"/>
+        <c:axId val="64360832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="60340096"/>
+        <c:crossAx val="64362368"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="60340096"/>
+        <c:axId val="64362368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2842,7 +2852,7 @@
         <c:axPos val="l"/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="60338560"/>
+        <c:crossAx val="64360832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2854,7 +2864,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000189" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000189" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000266" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000266" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3041,25 +3051,25 @@
           </c:val>
         </c:ser>
         <c:shape val="box"/>
-        <c:axId val="60353536"/>
-        <c:axId val="60355328"/>
+        <c:axId val="64380288"/>
+        <c:axId val="64386176"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="60353536"/>
+        <c:axId val="64380288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="60355328"/>
+        <c:crossAx val="64386176"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="60355328"/>
+        <c:axId val="64386176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3067,7 +3077,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="60353536"/>
+        <c:crossAx val="64380288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3079,7 +3089,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000189" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000189" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000266" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000266" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3376,7 +3386,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000133" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000133" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000211" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000211" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3402,7 +3412,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -3487,23 +3496,23 @@
           </c:bubbleSize>
         </c:ser>
         <c:bubbleScale val="100"/>
-        <c:axId val="71493504"/>
-        <c:axId val="71495040"/>
+        <c:axId val="64681856"/>
+        <c:axId val="64683392"/>
       </c:bubbleChart>
       <c:valAx>
-        <c:axId val="71493504"/>
+        <c:axId val="64681856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="71495040"/>
+        <c:crossAx val="64683392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="71495040"/>
+        <c:axId val="64683392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3511,20 +3520,19 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="71493504"/>
+        <c:crossAx val="64681856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000167" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000167" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3788,24 +3796,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="72496256"/>
-        <c:axId val="72497792"/>
+        <c:axId val="64742528"/>
+        <c:axId val="64744064"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="72496256"/>
+        <c:axId val="64742528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="72497792"/>
+        <c:crossAx val="64744064"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="72497792"/>
+        <c:axId val="64744064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3813,7 +3821,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="72496256"/>
+        <c:crossAx val="64742528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3825,7 +3833,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000189" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000189" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3836,15 +3844,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>133350</xdr:colOff>
+      <xdr:colOff>133349</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>438150</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:colOff>581024</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3908,8 +3916,8 @@
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>542925</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3936,10 +3944,10 @@
       <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>561975</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3965,14 +3973,14 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>19049</xdr:colOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>285749</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>133350</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
@@ -3995,16 +4003,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>228599</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>323850</xdr:colOff>
+      <xdr:colOff>200024</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4100,16 +4108,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>352425</xdr:colOff>
+      <xdr:colOff>304800</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4172,9 +4180,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>438150</xdr:colOff>
+      <xdr:colOff>304800</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>104774</xdr:rowOff>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4202,9 +4210,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>247650</xdr:colOff>
+      <xdr:colOff>9525</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4233,13 +4241,13 @@
       <xdr:col>1</xdr:col>
       <xdr:colOff>19050</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:rowOff>19049</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>323850</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>180974</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4583,8 +4591,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K23" sqref="K23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I18" sqref="H18:I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4599,7 +4607,7 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4862,7 +4870,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M23" sqref="M23"/>
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4891,7 +4899,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
@@ -4978,7 +4986,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="T7" sqref="T7"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4993,7 +5001,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
add a chart locating in one column and one row test
</commit_message>
<xml_diff>
--- a/zss-ngmodel/src/test/java/org/zkoss/zss/ngmodel/book/chart.xlsx
+++ b/zss-ngmodel/src/test/java/org/zkoss/zss/ngmodel/book/chart.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="44">
   <si>
     <t>Internet Explorer</t>
   </si>
@@ -151,6 +151,9 @@
   </si>
   <si>
     <t>6-Jan-07</t>
+  </si>
+  <si>
+    <t>Chart in the same column and row test</t>
   </si>
 </sst>
 </file>
@@ -590,24 +593,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="70504832"/>
-        <c:axId val="70506752"/>
+        <c:axId val="87039360"/>
+        <c:axId val="88130688"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="70504832"/>
+        <c:axId val="87039360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="70506752"/>
+        <c:crossAx val="88130688"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="70506752"/>
+        <c:axId val="88130688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -615,7 +618,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="70504832"/>
+        <c:crossAx val="87039360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -628,7 +631,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000244" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000244" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000266" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000266" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -907,26 +910,26 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="64761856"/>
-        <c:axId val="64763392"/>
-        <c:axId val="75238912"/>
+        <c:axId val="64794624"/>
+        <c:axId val="64796160"/>
+        <c:axId val="64786880"/>
       </c:line3DChart>
       <c:catAx>
-        <c:axId val="64761856"/>
+        <c:axId val="64794624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64763392"/>
+        <c:crossAx val="64796160"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="64763392"/>
+        <c:axId val="64796160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -940,19 +943,19 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="64761856"/>
+        <c:crossAx val="64794624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:serAx>
-        <c:axId val="75238912"/>
+        <c:axId val="64786880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="1"/>
         <c:axPos val="b"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="64763392"/>
+        <c:crossAx val="64796160"/>
         <c:crosses val="autoZero"/>
       </c:serAx>
     </c:plotArea>
@@ -963,7 +966,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000211" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000211" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000233" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000233" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1044,7 +1047,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000167" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000167" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000189" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000189" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1128,7 +1131,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000189" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000189" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000211" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000211" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1397,22 +1400,22 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="67547904"/>
-        <c:axId val="67549440"/>
+        <c:axId val="67609344"/>
+        <c:axId val="67610880"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="67547904"/>
+        <c:axId val="67609344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="67549440"/>
+        <c:crossAx val="67610880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="67549440"/>
+        <c:axId val="67610880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1420,7 +1423,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="67547904"/>
+        <c:crossAx val="67609344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1432,7 +1435,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000189" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000189" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000211" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000211" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1756,24 +1759,24 @@
           <c:upBars/>
           <c:downBars/>
         </c:upDownBars>
-        <c:axId val="69940352"/>
-        <c:axId val="69941888"/>
+        <c:axId val="70075520"/>
+        <c:axId val="70077056"/>
       </c:stockChart>
       <c:catAx>
-        <c:axId val="69940352"/>
+        <c:axId val="70075520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="69941888"/>
+        <c:crossAx val="70077056"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="69941888"/>
+        <c:axId val="70077056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1781,7 +1784,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="69940352"/>
+        <c:crossAx val="70075520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1793,7 +1796,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000155" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000155" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000178" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000178" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2053,26 +2056,26 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="72437760"/>
-        <c:axId val="72439296"/>
-        <c:axId val="70380160"/>
+        <c:axId val="64207488"/>
+        <c:axId val="64209280"/>
+        <c:axId val="72446848"/>
       </c:area3DChart>
       <c:catAx>
-        <c:axId val="72437760"/>
+        <c:axId val="64207488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="72439296"/>
+        <c:crossAx val="64209280"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="72439296"/>
+        <c:axId val="64209280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2081,19 +2084,19 @@
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="72437760"/>
+        <c:crossAx val="64207488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:serAx>
-        <c:axId val="70380160"/>
+        <c:axId val="72446848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="1"/>
         <c:axPos val="b"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="72439296"/>
+        <c:crossAx val="64209280"/>
         <c:crosses val="autoZero"/>
       </c:serAx>
     </c:plotArea>
@@ -2105,7 +2108,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000266" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000266" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000289" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000289" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2131,7 +2134,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -2288,11 +2290,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="88132608"/>
-        <c:axId val="64222336"/>
+        <c:axId val="64306176"/>
+        <c:axId val="64312448"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="88132608"/>
+        <c:axId val="64306176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2313,17 +2315,16 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64222336"/>
+        <c:crossAx val="64312448"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="64222336"/>
+        <c:axId val="64312448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2345,24 +2346,22 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="88132608"/>
+        <c:crossAx val="64306176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000278" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000278" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000003" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000003" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup orientation="portrait"/>
   </c:printSettings>
 </c:chartSpace>
@@ -2388,7 +2387,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
     </c:title>
     <c:view3D>
       <c:perspective val="30"/>
@@ -2599,25 +2597,25 @@
           </c:val>
         </c:ser>
         <c:shape val="box"/>
-        <c:axId val="64307200"/>
-        <c:axId val="64308736"/>
+        <c:axId val="64331776"/>
+        <c:axId val="64333312"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="64307200"/>
+        <c:axId val="64331776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64308736"/>
+        <c:crossAx val="64333312"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="64308736"/>
+        <c:axId val="64333312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2625,20 +2623,19 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64307200"/>
+        <c:crossAx val="64331776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000003" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000003" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000322" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000322" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup orientation="portrait"/>
   </c:printSettings>
 </c:chartSpace>
@@ -2826,25 +2823,25 @@
           <c:showVal val="1"/>
         </c:dLbls>
         <c:overlap val="-25"/>
-        <c:axId val="64360832"/>
-        <c:axId val="64362368"/>
+        <c:axId val="64393600"/>
+        <c:axId val="64395136"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="64360832"/>
+        <c:axId val="64393600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64362368"/>
+        <c:crossAx val="64395136"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="64362368"/>
+        <c:axId val="64395136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2852,7 +2849,7 @@
         <c:axPos val="l"/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="64360832"/>
+        <c:crossAx val="64393600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2864,7 +2861,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000266" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000266" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000289" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000289" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3051,25 +3048,25 @@
           </c:val>
         </c:ser>
         <c:shape val="box"/>
-        <c:axId val="64380288"/>
-        <c:axId val="64386176"/>
+        <c:axId val="64408960"/>
+        <c:axId val="64414848"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="64380288"/>
+        <c:axId val="64408960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64386176"/>
+        <c:crossAx val="64414848"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="64386176"/>
+        <c:axId val="64414848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3077,7 +3074,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64380288"/>
+        <c:crossAx val="64408960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3089,7 +3086,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000266" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000266" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000289" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000289" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3386,7 +3383,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000211" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000211" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000233" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000233" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3496,23 +3493,23 @@
           </c:bubbleSize>
         </c:ser>
         <c:bubbleScale val="100"/>
-        <c:axId val="64681856"/>
-        <c:axId val="64683392"/>
+        <c:axId val="64739200"/>
+        <c:axId val="64740736"/>
       </c:bubbleChart>
       <c:valAx>
-        <c:axId val="64681856"/>
+        <c:axId val="64739200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64683392"/>
+        <c:crossAx val="64740736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="64683392"/>
+        <c:axId val="64740736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3520,7 +3517,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64681856"/>
+        <c:crossAx val="64739200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3532,7 +3529,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000167" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000167" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000189" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000189" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3796,24 +3793,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="64742528"/>
-        <c:axId val="64744064"/>
+        <c:axId val="64775296"/>
+        <c:axId val="64776832"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="64742528"/>
+        <c:axId val="64775296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64744064"/>
+        <c:crossAx val="64776832"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="64744064"/>
+        <c:axId val="64776832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3821,7 +3818,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64742528"/>
+        <c:crossAx val="64775296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3833,7 +3830,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000189" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000189" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000211" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000211" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3844,15 +3841,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>133349</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:colOff>209549</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>114301</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>581024</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>4905375</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>2809875</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3873,16 +3870,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>476249</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>257174</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:rowOff>133351</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>428624</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>209549</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>104776</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4589,14 +4586,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I18" sqref="H18:I18"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="77.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="27.75" customHeight="1">
+      <c r="A1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="236.25" customHeight="1"/>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
add a title for each chart
</commit_message>
<xml_diff>
--- a/zss-ngmodel/src/test/java/org/zkoss/zss/ngmodel/book/chart.xlsx
+++ b/zss-ngmodel/src/test/java/org/zkoss/zss/ngmodel/book/chart.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="345" windowWidth="17955" windowHeight="7455"/>
+    <workbookView xWindow="600" yWindow="345" windowWidth="17955" windowHeight="7455" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Area" sheetId="3" r:id="rId1"/>
@@ -349,6 +349,25 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Area</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="1"/>
+    </c:title>
     <c:plotArea>
       <c:layout/>
       <c:areaChart>
@@ -593,24 +612,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="87039360"/>
-        <c:axId val="88130688"/>
+        <c:axId val="122695040"/>
+        <c:axId val="122722176"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="87039360"/>
+        <c:axId val="122695040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="88130688"/>
+        <c:crossAx val="122722176"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="88130688"/>
+        <c:axId val="122722176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -618,7 +637,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87039360"/>
+        <c:crossAx val="122695040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -631,7 +650,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000266" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000266" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000278" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000278" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -662,6 +681,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
     </c:title>
     <c:view3D>
       <c:perspective val="30"/>
@@ -910,26 +930,26 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="64794624"/>
-        <c:axId val="64796160"/>
-        <c:axId val="64786880"/>
+        <c:axId val="107244928"/>
+        <c:axId val="107263104"/>
+        <c:axId val="107237376"/>
       </c:line3DChart>
       <c:catAx>
-        <c:axId val="64794624"/>
+        <c:axId val="107244928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64796160"/>
+        <c:crossAx val="107263104"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="64796160"/>
+        <c:axId val="107263104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -943,30 +963,31 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="64794624"/>
+        <c:crossAx val="107244928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:serAx>
-        <c:axId val="64786880"/>
+        <c:axId val="107237376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="1"/>
         <c:axPos val="b"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="64796160"/>
+        <c:crossAx val="107263104"/>
         <c:crosses val="autoZero"/>
       </c:serAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000233" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000233" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000244" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000244" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1042,12 +1063,13 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000189" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000189" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000002" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000002" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1126,12 +1148,13 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000211" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000211" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000222" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000222" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1141,6 +1164,24 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Scatter Chart Title</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
@@ -1400,22 +1441,22 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="67609344"/>
-        <c:axId val="67610880"/>
+        <c:axId val="107884928"/>
+        <c:axId val="107886464"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="67609344"/>
+        <c:axId val="107884928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="67610880"/>
+        <c:crossAx val="107886464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="67610880"/>
+        <c:axId val="107886464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1423,19 +1464,20 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="67609344"/>
+        <c:crossAx val="107884928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000211" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000211" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000222" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000222" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1446,6 +1488,24 @@
   <c:lang val="en-US"/>
   <c:style val="4"/>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Stock Chart Title</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
     <c:plotArea>
       <c:layout/>
       <c:stockChart>
@@ -1759,24 +1819,24 @@
           <c:upBars/>
           <c:downBars/>
         </c:upDownBars>
-        <c:axId val="70075520"/>
-        <c:axId val="70077056"/>
+        <c:axId val="107901696"/>
+        <c:axId val="107903232"/>
       </c:stockChart>
       <c:catAx>
-        <c:axId val="70075520"/>
+        <c:axId val="107901696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="70077056"/>
+        <c:crossAx val="107903232"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="70077056"/>
+        <c:axId val="107903232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1784,19 +1844,20 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="70075520"/>
+        <c:crossAx val="107901696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000178" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000178" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000189" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000189" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1807,6 +1868,21 @@
   <c:lang val="en-US"/>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Area 3D</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
     </c:title>
     <c:view3D>
@@ -2056,26 +2132,26 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="64207488"/>
-        <c:axId val="64209280"/>
-        <c:axId val="72446848"/>
+        <c:axId val="98453376"/>
+        <c:axId val="98454912"/>
+        <c:axId val="98937920"/>
       </c:area3DChart>
       <c:catAx>
-        <c:axId val="64207488"/>
+        <c:axId val="98453376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64209280"/>
+        <c:crossAx val="98454912"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="64209280"/>
+        <c:axId val="98454912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2084,19 +2160,19 @@
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64207488"/>
+        <c:crossAx val="98453376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:serAx>
-        <c:axId val="72446848"/>
+        <c:axId val="98937920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="1"/>
         <c:axPos val="b"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="64209280"/>
+        <c:crossAx val="98454912"/>
         <c:crosses val="autoZero"/>
       </c:serAx>
     </c:plotArea>
@@ -2108,7 +2184,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000289" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000289" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000003" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000003" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2134,6 +2210,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -2290,11 +2367,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="64306176"/>
-        <c:axId val="64312448"/>
+        <c:axId val="98658560"/>
+        <c:axId val="98660736"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="64306176"/>
+        <c:axId val="98658560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2315,16 +2392,17 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64312448"/>
+        <c:crossAx val="98660736"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="64312448"/>
+        <c:axId val="98660736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2346,22 +2424,24 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64306176"/>
+        <c:crossAx val="98658560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000003" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000003" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000311" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000311" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup orientation="portrait"/>
   </c:printSettings>
 </c:chartSpace>
@@ -2387,6 +2467,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
     </c:title>
     <c:view3D>
       <c:perspective val="30"/>
@@ -2597,25 +2678,25 @@
           </c:val>
         </c:ser>
         <c:shape val="box"/>
-        <c:axId val="64331776"/>
-        <c:axId val="64333312"/>
+        <c:axId val="98688000"/>
+        <c:axId val="98910976"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="64331776"/>
+        <c:axId val="98688000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64333312"/>
+        <c:crossAx val="98910976"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="64333312"/>
+        <c:axId val="98910976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2623,19 +2704,20 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64331776"/>
+        <c:crossAx val="98688000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000322" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000322" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000333" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000333" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup orientation="portrait"/>
   </c:printSettings>
 </c:chartSpace>
@@ -2645,7 +2727,24 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
-    <c:title/>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Column Title</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
@@ -2823,25 +2922,25 @@
           <c:showVal val="1"/>
         </c:dLbls>
         <c:overlap val="-25"/>
-        <c:axId val="64393600"/>
-        <c:axId val="64395136"/>
+        <c:axId val="98930048"/>
+        <c:axId val="104535168"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="64393600"/>
+        <c:axId val="98930048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64395136"/>
+        <c:crossAx val="104535168"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="64395136"/>
+        <c:axId val="104535168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2849,19 +2948,20 @@
         <c:axPos val="l"/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="64393600"/>
+        <c:crossAx val="98930048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000289" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000289" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000003" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000003" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2871,6 +2971,25 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" b="1" i="0" baseline="0"/>
+              <a:t>Column 3D Title</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
     <c:view3D>
       <c:rAngAx val="1"/>
     </c:view3D>
@@ -3048,25 +3167,25 @@
           </c:val>
         </c:ser>
         <c:shape val="box"/>
-        <c:axId val="64408960"/>
-        <c:axId val="64414848"/>
+        <c:axId val="104548992"/>
+        <c:axId val="104554880"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="64408960"/>
+        <c:axId val="104548992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64414848"/>
+        <c:crossAx val="104554880"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="64414848"/>
+        <c:axId val="104554880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3074,19 +3193,20 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64408960"/>
+        <c:crossAx val="104548992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000289" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000289" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000003" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000003" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3112,6 +3232,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -3378,12 +3499,13 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000233" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000233" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000244" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000244" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3409,6 +3531,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -3493,23 +3616,23 @@
           </c:bubbleSize>
         </c:ser>
         <c:bubbleScale val="100"/>
-        <c:axId val="64739200"/>
-        <c:axId val="64740736"/>
+        <c:axId val="106092032"/>
+        <c:axId val="106093568"/>
       </c:bubbleChart>
       <c:valAx>
-        <c:axId val="64739200"/>
+        <c:axId val="106092032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64740736"/>
+        <c:crossAx val="106093568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="64740736"/>
+        <c:axId val="106093568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3517,19 +3640,20 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64739200"/>
+        <c:crossAx val="106092032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000189" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000189" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000002" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000002" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3539,6 +3663,24 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Line Title</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
@@ -3793,24 +3935,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="64775296"/>
-        <c:axId val="64776832"/>
+        <c:axId val="106873600"/>
+        <c:axId val="106875136"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="64775296"/>
+        <c:axId val="106873600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64776832"/>
+        <c:crossAx val="106875136"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="64776832"/>
+        <c:axId val="106875136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3818,19 +3960,20 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64775296"/>
+        <c:crossAx val="106873600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000211" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000211" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000222" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000222" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4588,7 +4731,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
@@ -4877,7 +5020,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+      <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5094,8 +5237,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O26" sqref="O26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
* import bar, line, pie, scatter chart * comment out set legend position for we get incorrect value * add a new scatter chart with numeric x axis values
</commit_message>
<xml_diff>
--- a/zss-ngmodel/src/test/java/org/zkoss/zss/ngmodel/book/chart.xlsx
+++ b/zss-ngmodel/src/test/java/org/zkoss/zss/ngmodel/book/chart.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="345" windowWidth="17955" windowHeight="7455" activeTab="8"/>
+    <workbookView xWindow="600" yWindow="345" windowWidth="17955" windowHeight="7455" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Area" sheetId="3" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="47">
   <si>
     <t>Internet Explorer</t>
   </si>
@@ -154,6 +154,15 @@
   </si>
   <si>
     <t>Chart in the same column and row test</t>
+  </si>
+  <si>
+    <t>Series name is string literal</t>
+  </si>
+  <si>
+    <t>Daily Ranfall</t>
+  </si>
+  <si>
+    <t>Particulate</t>
   </si>
 </sst>
 </file>
@@ -365,7 +374,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="1"/>
     </c:title>
     <c:plotArea>
@@ -612,24 +620,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="122695040"/>
-        <c:axId val="122722176"/>
+        <c:axId val="72750976"/>
+        <c:axId val="72752512"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="122695040"/>
+        <c:axId val="72750976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="122722176"/>
+        <c:crossAx val="72752512"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="122722176"/>
+        <c:axId val="72752512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -637,20 +645,19 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="122695040"/>
+        <c:crossAx val="72750976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000278" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000278" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000003" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000003" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -930,26 +937,26 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="107244928"/>
-        <c:axId val="107263104"/>
-        <c:axId val="107237376"/>
+        <c:axId val="59725312"/>
+        <c:axId val="59726848"/>
+        <c:axId val="140103168"/>
       </c:line3DChart>
       <c:catAx>
-        <c:axId val="107244928"/>
+        <c:axId val="59725312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="107263104"/>
+        <c:crossAx val="59726848"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="107263104"/>
+        <c:axId val="59726848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -963,19 +970,19 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="107244928"/>
+        <c:crossAx val="59725312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:serAx>
-        <c:axId val="107237376"/>
+        <c:axId val="140103168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="1"/>
         <c:axPos val="b"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="107263104"/>
+        <c:crossAx val="59726848"/>
         <c:crosses val="autoZero"/>
       </c:serAx>
     </c:plotArea>
@@ -987,7 +994,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000244" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000244" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000266" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000266" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1069,7 +1076,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000002" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000002" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000222" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000222" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1154,7 +1161,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000222" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000222" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000244" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000244" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1441,22 +1448,23 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="107884928"/>
-        <c:axId val="107886464"/>
+        <c:axId val="61675776"/>
+        <c:axId val="61685760"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="107884928"/>
+        <c:axId val="61675776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="107886464"/>
+        <c:crossAx val="61685760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="107886464"/>
+        <c:axId val="61685760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1464,7 +1472,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="107884928"/>
+        <c:crossAx val="61675776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1477,13 +1485,159 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000222" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000222" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000244" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000244" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Scatter!$B$18</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Particulate</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Scatter!$A$19:$A$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>4.0999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7.3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Scatter!$B$19:$B$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>122</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>117</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>112</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>114</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>114</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>137</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>104</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:axId val="72081792"/>
+        <c:axId val="72080000"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="72081792"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="72080000"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="72080000"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="72081792"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:style val="4"/>
@@ -1564,22 +1718,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>27.2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>25.03</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>19.05</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>20.329999999999998</c:v>
+                  <c:v>30.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>35.03</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>39.049999999999997</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30.33</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>18.559999999999999</c:v>
+                  <c:v>28.7</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>18.559999999999999</c:v>
+                  <c:v>28.6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1655,7 +1809,7 @@
                   <c:v>18.559999999999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>18.559999999999999</c:v>
+                  <c:v>13.56</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1731,7 +1885,7 @@
                   <c:v>16.329999999999998</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>16.329999999999998</c:v>
+                  <c:v>12.33</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1807,7 +1961,7 @@
                   <c:v>17.350000000000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>17.350000000000001</c:v>
+                  <c:v>13.35</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1819,24 +1973,24 @@
           <c:upBars/>
           <c:downBars/>
         </c:upDownBars>
-        <c:axId val="107901696"/>
-        <c:axId val="107903232"/>
+        <c:axId val="61733888"/>
+        <c:axId val="72098560"/>
       </c:stockChart>
       <c:catAx>
-        <c:axId val="107901696"/>
+        <c:axId val="61733888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="107903232"/>
+        <c:crossAx val="72098560"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="107903232"/>
+        <c:axId val="72098560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1844,7 +1998,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="107901696"/>
+        <c:crossAx val="61733888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1857,7 +2011,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000189" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000189" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000211" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000211" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1883,7 +2037,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
     </c:title>
     <c:view3D>
       <c:perspective val="30"/>
@@ -2132,26 +2285,26 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="98453376"/>
-        <c:axId val="98454912"/>
-        <c:axId val="98937920"/>
+        <c:axId val="87774720"/>
+        <c:axId val="88210048"/>
+        <c:axId val="74228608"/>
       </c:area3DChart>
       <c:catAx>
-        <c:axId val="98453376"/>
+        <c:axId val="87774720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="98454912"/>
+        <c:crossAx val="88210048"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="98454912"/>
+        <c:axId val="88210048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2160,31 +2313,30 @@
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="98453376"/>
+        <c:crossAx val="87774720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:serAx>
-        <c:axId val="98937920"/>
+        <c:axId val="74228608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="1"/>
         <c:axPos val="b"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="98454912"/>
+        <c:crossAx val="88210048"/>
         <c:crosses val="autoZero"/>
       </c:serAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000003" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000003" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000322" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000322" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2210,7 +2362,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -2367,11 +2518,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="98658560"/>
-        <c:axId val="98660736"/>
+        <c:axId val="59355136"/>
+        <c:axId val="59357056"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="98658560"/>
+        <c:axId val="59355136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2392,17 +2543,16 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="98660736"/>
+        <c:crossAx val="59357056"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="98660736"/>
+        <c:axId val="59357056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2424,24 +2574,22 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="98658560"/>
+        <c:crossAx val="59355136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000311" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000311" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000333" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000333" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup orientation="portrait"/>
   </c:printSettings>
 </c:chartSpace>
@@ -2467,7 +2615,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
     </c:title>
     <c:view3D>
       <c:perspective val="30"/>
@@ -2678,25 +2825,25 @@
           </c:val>
         </c:ser>
         <c:shape val="box"/>
-        <c:axId val="98688000"/>
-        <c:axId val="98910976"/>
+        <c:axId val="59368192"/>
+        <c:axId val="59369728"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="98688000"/>
+        <c:axId val="59368192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="98910976"/>
+        <c:crossAx val="59369728"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="98910976"/>
+        <c:axId val="59369728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2704,20 +2851,19 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="98688000"/>
+        <c:crossAx val="59368192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000333" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000333" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000355" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000355" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup orientation="portrait"/>
   </c:printSettings>
 </c:chartSpace>
@@ -2743,7 +2889,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -2922,25 +3067,25 @@
           <c:showVal val="1"/>
         </c:dLbls>
         <c:overlap val="-25"/>
-        <c:axId val="98930048"/>
-        <c:axId val="104535168"/>
+        <c:axId val="59524224"/>
+        <c:axId val="59525760"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="98930048"/>
+        <c:axId val="59524224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="104535168"/>
+        <c:crossAx val="59525760"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="104535168"/>
+        <c:axId val="59525760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2948,20 +3093,19 @@
         <c:axPos val="l"/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="98930048"/>
+        <c:crossAx val="59524224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000003" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000003" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000322" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000322" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2988,7 +3132,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
     </c:title>
     <c:view3D>
       <c:rAngAx val="1"/>
@@ -3167,25 +3310,25 @@
           </c:val>
         </c:ser>
         <c:shape val="box"/>
-        <c:axId val="104548992"/>
-        <c:axId val="104554880"/>
+        <c:axId val="59535744"/>
+        <c:axId val="59537280"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="104548992"/>
+        <c:axId val="59535744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="104554880"/>
+        <c:crossAx val="59537280"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="104554880"/>
+        <c:axId val="59537280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3193,20 +3336,19 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="104548992"/>
+        <c:crossAx val="59535744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000003" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000003" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000322" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000322" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3232,7 +3374,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -3499,13 +3640,12 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000244" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000244" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000266" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000266" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3531,7 +3671,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -3616,23 +3755,23 @@
           </c:bubbleSize>
         </c:ser>
         <c:bubbleScale val="100"/>
-        <c:axId val="106092032"/>
-        <c:axId val="106093568"/>
+        <c:axId val="59624448"/>
+        <c:axId val="59642624"/>
       </c:bubbleChart>
       <c:valAx>
-        <c:axId val="106092032"/>
+        <c:axId val="59624448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106093568"/>
+        <c:crossAx val="59642624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="106093568"/>
+        <c:axId val="59642624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3640,20 +3779,19 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106092032"/>
+        <c:crossAx val="59624448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000002" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000002" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000222" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000222" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3935,24 +4073,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="106873600"/>
-        <c:axId val="106875136"/>
+        <c:axId val="59701504"/>
+        <c:axId val="59711488"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="106873600"/>
+        <c:axId val="59701504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106875136"/>
+        <c:crossAx val="59711488"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="106875136"/>
+        <c:axId val="59711488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3960,7 +4098,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106873600"/>
+        <c:crossAx val="59701504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3973,7 +4111,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000222" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000222" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000244" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000244" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4378,16 +4516,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>3</xdr:col>
       <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>19049</xdr:rowOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>180974</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>66676</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4401,6 +4539,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -5148,10 +5316,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+      <selection activeCell="A19" sqref="A19:C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5212,6 +5380,11 @@
         <v>3.24</v>
       </c>
     </row>
+    <row r="19" spans="3:3">
+      <c r="C19" t="s">
+        <v>44</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5220,16 +5393,102 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A18:B27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18:B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="18" spans="1:2">
+      <c r="A18" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="B19">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20">
+        <v>4.3</v>
+      </c>
+      <c r="B20">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21">
+        <v>5.7</v>
+      </c>
+      <c r="B21">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22">
+        <v>5.4</v>
+      </c>
+      <c r="B22">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23">
+        <v>5.9</v>
+      </c>
+      <c r="B23">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24">
+        <v>5</v>
+      </c>
+      <c r="B24">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25">
+        <v>3.6</v>
+      </c>
+      <c r="B25">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26">
+        <v>1.9</v>
+      </c>
+      <c r="B26">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27">
+        <v>7.3</v>
+      </c>
+      <c r="B27">
+        <v>104</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -5237,8 +5496,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O26" sqref="O26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5286,7 +5545,7 @@
         <v>37</v>
       </c>
       <c r="B3" s="10">
-        <v>27.2</v>
+        <v>30.2</v>
       </c>
       <c r="C3" s="10">
         <v>27.2</v>
@@ -5306,7 +5565,7 @@
         <v>38</v>
       </c>
       <c r="B4" s="9">
-        <v>25.03</v>
+        <v>35.03</v>
       </c>
       <c r="C4" s="9">
         <v>25.03</v>
@@ -5326,7 +5585,7 @@
         <v>39</v>
       </c>
       <c r="B5" s="10">
-        <v>19.05</v>
+        <v>39.049999999999997</v>
       </c>
       <c r="C5" s="10">
         <v>19.05</v>
@@ -5346,7 +5605,7 @@
         <v>40</v>
       </c>
       <c r="B6" s="9">
-        <v>20.329999999999998</v>
+        <v>30.33</v>
       </c>
       <c r="C6" s="9">
         <v>20.329999999999998</v>
@@ -5366,7 +5625,7 @@
         <v>41</v>
       </c>
       <c r="B7" s="10">
-        <v>18.559999999999999</v>
+        <v>28.7</v>
       </c>
       <c r="C7" s="10">
         <v>18.559999999999999</v>
@@ -5386,19 +5645,19 @@
         <v>42</v>
       </c>
       <c r="B8" s="10">
-        <v>18.559999999999999</v>
+        <v>28.6</v>
       </c>
       <c r="C8" s="10">
-        <v>18.559999999999999</v>
+        <v>13.56</v>
       </c>
       <c r="D8" s="10">
-        <v>16.329999999999998</v>
+        <v>12.33</v>
       </c>
       <c r="E8" s="10">
-        <v>17.350000000000001</v>
+        <v>13.35</v>
       </c>
       <c r="F8" s="11">
-        <v>25895</v>
+        <v>22895</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
* change bubble chart test data to display more clearly * set fixed legend position for we cannot get correct value from POI
</commit_message>
<xml_diff>
--- a/zss-ngmodel/src/test/java/org/zkoss/zss/ngmodel/book/chart.xlsx
+++ b/zss-ngmodel/src/test/java/org/zkoss/zss/ngmodel/book/chart.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="345" windowWidth="17955" windowHeight="7455" activeTab="7"/>
+    <workbookView xWindow="600" yWindow="345" windowWidth="17955" windowHeight="7455" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Area" sheetId="3" r:id="rId1"/>
@@ -81,15 +81,6 @@
     <t>Month</t>
   </si>
   <si>
-    <t>Number of Products</t>
-  </si>
-  <si>
-    <t>Sales</t>
-  </si>
-  <si>
-    <t>Market Share</t>
-  </si>
-  <si>
     <t>Browser market share 2013</t>
   </si>
   <si>
@@ -163,6 +154,15 @@
   </si>
   <si>
     <t>Particulate</t>
+  </si>
+  <si>
+    <t>Y values</t>
+  </si>
+  <si>
+    <t>X values</t>
+  </si>
+  <si>
+    <t>Z values</t>
   </si>
 </sst>
 </file>
@@ -317,7 +317,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -325,7 +325,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -620,24 +619,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="72750976"/>
-        <c:axId val="72752512"/>
+        <c:axId val="11401856"/>
+        <c:axId val="50676096"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="72750976"/>
+        <c:axId val="11401856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="72752512"/>
+        <c:crossAx val="50676096"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="72752512"/>
+        <c:axId val="50676096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -645,7 +644,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="72750976"/>
+        <c:crossAx val="11401856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -657,7 +656,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000003" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000003" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000311" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000311" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -688,7 +687,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
     </c:title>
     <c:view3D>
       <c:perspective val="30"/>
@@ -937,26 +935,26 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="59725312"/>
-        <c:axId val="59726848"/>
-        <c:axId val="140103168"/>
+        <c:axId val="59961344"/>
+        <c:axId val="59962880"/>
+        <c:axId val="59919872"/>
       </c:line3DChart>
       <c:catAx>
-        <c:axId val="59725312"/>
+        <c:axId val="59961344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="59726848"/>
+        <c:crossAx val="59962880"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="59726848"/>
+        <c:axId val="59962880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -970,31 +968,30 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="59725312"/>
+        <c:crossAx val="59961344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:serAx>
-        <c:axId val="140103168"/>
+        <c:axId val="59919872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="1"/>
         <c:axPos val="b"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="59726848"/>
+        <c:crossAx val="59962880"/>
         <c:crosses val="autoZero"/>
       </c:serAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000266" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000266" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000278" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000278" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1070,13 +1067,12 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000222" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000222" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000233" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000233" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1155,13 +1151,12 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000244" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000244" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000255" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000255" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1448,23 +1443,23 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="61675776"/>
-        <c:axId val="61685760"/>
+        <c:axId val="61317888"/>
+        <c:axId val="61319424"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="61675776"/>
+        <c:axId val="61317888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="61685760"/>
+        <c:crossAx val="61319424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="61685760"/>
+        <c:axId val="61319424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1472,7 +1467,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="61675776"/>
+        <c:crossAx val="61317888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1485,7 +1480,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000244" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000244" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000255" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000255" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1594,23 +1589,23 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="72081792"/>
-        <c:axId val="72080000"/>
+        <c:axId val="61330944"/>
+        <c:axId val="61332480"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="72081792"/>
+        <c:axId val="61330944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="72080000"/>
+        <c:crossAx val="61332480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="72080000"/>
+        <c:axId val="61332480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1618,7 +1613,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="72081792"/>
+        <c:crossAx val="61330944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1631,7 +1626,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1658,7 +1653,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -1973,24 +1967,24 @@
           <c:upBars/>
           <c:downBars/>
         </c:upDownBars>
-        <c:axId val="61733888"/>
-        <c:axId val="72098560"/>
+        <c:axId val="61430400"/>
+        <c:axId val="61444480"/>
       </c:stockChart>
       <c:catAx>
-        <c:axId val="61733888"/>
+        <c:axId val="61430400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="72098560"/>
+        <c:crossAx val="61444480"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="72098560"/>
+        <c:axId val="61444480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1998,20 +1992,19 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="61733888"/>
+        <c:crossAx val="61430400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000211" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000211" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000222" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000222" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2285,26 +2278,26 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="87774720"/>
-        <c:axId val="88210048"/>
-        <c:axId val="74228608"/>
+        <c:axId val="55916416"/>
+        <c:axId val="55917952"/>
+        <c:axId val="58796672"/>
       </c:area3DChart>
       <c:catAx>
-        <c:axId val="87774720"/>
+        <c:axId val="55916416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="88210048"/>
+        <c:crossAx val="55917952"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="88210048"/>
+        <c:axId val="55917952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2313,19 +2306,19 @@
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87774720"/>
+        <c:crossAx val="55916416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:serAx>
-        <c:axId val="74228608"/>
+        <c:axId val="58796672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="1"/>
         <c:axPos val="b"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="88210048"/>
+        <c:crossAx val="55917952"/>
         <c:crosses val="autoZero"/>
       </c:serAx>
     </c:plotArea>
@@ -2336,7 +2329,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000322" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000322" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000333" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000333" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2518,11 +2511,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="59355136"/>
-        <c:axId val="59357056"/>
+        <c:axId val="58792192"/>
+        <c:axId val="58986880"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="59355136"/>
+        <c:axId val="58792192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2545,14 +2538,14 @@
           </c:tx>
         </c:title>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="59357056"/>
+        <c:crossAx val="58986880"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="59357056"/>
+        <c:axId val="58986880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2577,7 +2570,7 @@
         </c:title>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="59355136"/>
+        <c:crossAx val="58792192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2589,7 +2582,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000333" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000333" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000344" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000344" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup orientation="portrait"/>
   </c:printSettings>
 </c:chartSpace>
@@ -2825,25 +2818,25 @@
           </c:val>
         </c:ser>
         <c:shape val="box"/>
-        <c:axId val="59368192"/>
-        <c:axId val="59369728"/>
+        <c:axId val="59001856"/>
+        <c:axId val="59007744"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="59368192"/>
+        <c:axId val="59001856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="59369728"/>
+        <c:crossAx val="59007744"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="59369728"/>
+        <c:axId val="59007744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2851,7 +2844,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="59368192"/>
+        <c:crossAx val="59001856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2863,7 +2856,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000355" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000355" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000366" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000366" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup orientation="portrait"/>
   </c:printSettings>
 </c:chartSpace>
@@ -3067,25 +3060,25 @@
           <c:showVal val="1"/>
         </c:dLbls>
         <c:overlap val="-25"/>
-        <c:axId val="59524224"/>
-        <c:axId val="59525760"/>
+        <c:axId val="59084160"/>
+        <c:axId val="59098240"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="59524224"/>
+        <c:axId val="59084160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="59525760"/>
+        <c:crossAx val="59098240"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="59525760"/>
+        <c:axId val="59098240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3093,7 +3086,7 @@
         <c:axPos val="l"/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="59524224"/>
+        <c:crossAx val="59084160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3105,7 +3098,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000322" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000322" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000333" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000333" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3310,25 +3303,25 @@
           </c:val>
         </c:ser>
         <c:shape val="box"/>
-        <c:axId val="59535744"/>
-        <c:axId val="59537280"/>
+        <c:axId val="59128448"/>
+        <c:axId val="59134336"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="59535744"/>
+        <c:axId val="59128448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="59537280"/>
+        <c:crossAx val="59134336"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="59537280"/>
+        <c:axId val="59134336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3336,7 +3329,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="59535744"/>
+        <c:crossAx val="59128448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3348,7 +3341,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000322" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000322" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000333" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000333" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3645,7 +3638,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000266" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000266" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000278" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000278" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3671,6 +3664,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -3688,16 +3682,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="2">
                   <c:v>20</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>18</c:v>
+                <c:pt idx="1">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>22</c:v>
@@ -3712,19 +3706,19 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>5500</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>12200</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>60000</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>24400</c:v>
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>135</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>160</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>32000</c:v>
+                  <c:v>320</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3733,45 +3727,126 @@
             <c:numRef>
               <c:f>Bubble!$C$2:$C$6</c:f>
               <c:numCache>
-                <c:formatCode>0%</c:formatCode>
+                <c:formatCode>0</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.03</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.12</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.33</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.1</c:v>
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.42</c:v>
+                  <c:v>22</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:bubbleSize>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="25400">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Bubble!$A$8:$A$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Bubble!$B$8:$B$12</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>145</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>300</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:bubbleSize>
+            <c:numRef>
+              <c:f>Bubble!$C$8:$C$12</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:bubbleSize>
         </c:ser>
         <c:bubbleScale val="100"/>
-        <c:axId val="59624448"/>
-        <c:axId val="59642624"/>
+        <c:axId val="59880960"/>
+        <c:axId val="59882496"/>
       </c:bubbleChart>
       <c:valAx>
-        <c:axId val="59624448"/>
+        <c:axId val="59880960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="59642624"/>
+        <c:crossAx val="59882496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="59642624"/>
+        <c:axId val="59882496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3779,19 +3854,20 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="59624448"/>
+        <c:crossAx val="59880960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000222" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000222" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000233" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000233" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3817,7 +3893,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -4073,24 +4148,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="59701504"/>
-        <c:axId val="59711488"/>
+        <c:axId val="59933440"/>
+        <c:axId val="59934976"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="59701504"/>
+        <c:axId val="59933440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="59711488"/>
+        <c:crossAx val="59934976"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="59711488"/>
+        <c:axId val="59934976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4098,20 +4173,19 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="59701504"/>
+        <c:crossAx val="59933440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000244" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000244" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000255" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000255" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4910,7 +4984,7 @@
   <sheetData>
     <row r="1" spans="1:1" ht="27.75" customHeight="1">
       <c r="A1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="236.25" customHeight="1"/>
@@ -5215,10 +5289,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5226,59 +5300,59 @@
     <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="30">
-      <c r="A1" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>21</v>
+    <row r="1" spans="1:3">
+      <c r="A1" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="B2" s="4">
-        <v>5500</v>
-      </c>
-      <c r="C2" s="5">
-        <v>0.03</v>
+        <v>120</v>
+      </c>
+      <c r="C2" s="4">
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="B3" s="4">
-        <v>12200</v>
-      </c>
-      <c r="C3" s="5">
-        <v>0.12</v>
+        <v>135</v>
+      </c>
+      <c r="C3" s="4">
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="B4" s="4">
-        <v>60000</v>
-      </c>
-      <c r="C4" s="5">
-        <v>0.33</v>
+        <v>140</v>
+      </c>
+      <c r="C4" s="4">
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5">
-        <v>18</v>
+        <v>80</v>
       </c>
       <c r="B5" s="4">
-        <v>24400</v>
-      </c>
-      <c r="C5" s="5">
-        <v>0.1</v>
+        <v>160</v>
+      </c>
+      <c r="C5" s="4">
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -5286,10 +5360,65 @@
         <v>22</v>
       </c>
       <c r="B6" s="4">
-        <v>32000</v>
-      </c>
-      <c r="C6" s="5">
-        <v>0.42</v>
+        <v>320</v>
+      </c>
+      <c r="C6" s="4">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8">
+        <v>30</v>
+      </c>
+      <c r="B8" s="4">
+        <v>120</v>
+      </c>
+      <c r="C8" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9">
+        <v>50</v>
+      </c>
+      <c r="B9" s="4">
+        <v>130</v>
+      </c>
+      <c r="C9" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10">
+        <v>70</v>
+      </c>
+      <c r="B10" s="4">
+        <v>145</v>
+      </c>
+      <c r="C10" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11">
+        <v>90</v>
+      </c>
+      <c r="B11" s="4">
+        <v>180</v>
+      </c>
+      <c r="C11" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12">
+        <v>100</v>
+      </c>
+      <c r="B12" s="4">
+        <v>300</v>
+      </c>
+      <c r="C12" s="4">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -5328,8 +5457,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="6" t="s">
-        <v>22</v>
+      <c r="A1" s="5" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -5358,7 +5487,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B5">
         <v>9.07</v>
@@ -5366,7 +5495,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B6">
         <v>3.38</v>
@@ -5374,7 +5503,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B7">
         <v>3.24</v>
@@ -5382,7 +5511,7 @@
     </row>
     <row r="19" spans="3:3">
       <c r="C19" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -5395,7 +5524,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A18:B27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A29" workbookViewId="0">
       <selection activeCell="A18" sqref="A18:B27"/>
     </sheetView>
   </sheetViews>
@@ -5406,11 +5535,11 @@
   </cols>
   <sheetData>
     <row r="18" spans="1:2">
-      <c r="A18" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>46</v>
+      <c r="A18" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -5503,160 +5632,160 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:6" ht="17.25" thickBot="1">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="F1" s="8" t="s">
+      <c r="E1" s="7" t="s">
         <v>27</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="17.25" thickBot="1">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="D2" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>32</v>
+      <c r="F2" s="8" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="17.25" thickBot="1">
-      <c r="A3" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="B3" s="10">
+      <c r="A3" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="9">
         <v>30.2</v>
       </c>
-      <c r="C3" s="10">
+      <c r="C3" s="9">
         <v>27.2</v>
       </c>
-      <c r="D3" s="10">
+      <c r="D3" s="9">
         <v>23.49</v>
       </c>
-      <c r="E3" s="10">
+      <c r="E3" s="9">
         <v>25.45</v>
       </c>
-      <c r="F3" s="11">
+      <c r="F3" s="10">
         <v>41301</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="17.25" thickBot="1">
-      <c r="A4" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="B4" s="9">
+      <c r="A4" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="8">
         <v>35.03</v>
       </c>
-      <c r="C4" s="9">
+      <c r="C4" s="8">
         <v>25.03</v>
       </c>
-      <c r="D4" s="9">
+      <c r="D4" s="8">
         <v>19.55</v>
       </c>
-      <c r="E4" s="9">
+      <c r="E4" s="8">
         <v>23.05</v>
       </c>
-      <c r="F4" s="12">
+      <c r="F4" s="11">
         <v>35203</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="17.25" thickBot="1">
-      <c r="A5" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="B5" s="10">
+      <c r="A5" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" s="9">
         <v>39.049999999999997</v>
       </c>
-      <c r="C5" s="10">
+      <c r="C5" s="9">
         <v>19.05</v>
       </c>
-      <c r="D5" s="10">
+      <c r="D5" s="9">
         <v>15.12</v>
       </c>
-      <c r="E5" s="10">
+      <c r="E5" s="9">
         <v>17.32</v>
       </c>
-      <c r="F5" s="11">
+      <c r="F5" s="10">
         <v>27908</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="17.25" thickBot="1">
-      <c r="A6" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="B6" s="9">
+      <c r="A6" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" s="8">
         <v>30.33</v>
       </c>
-      <c r="C6" s="9">
+      <c r="C6" s="8">
         <v>20.329999999999998</v>
       </c>
-      <c r="D6" s="9">
+      <c r="D6" s="8">
         <v>17.84</v>
       </c>
-      <c r="E6" s="9">
+      <c r="E6" s="8">
         <v>20.45</v>
       </c>
-      <c r="F6" s="12">
+      <c r="F6" s="11">
         <v>29567</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="17.25" thickBot="1">
-      <c r="A7" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="B7" s="10">
+      <c r="A7" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" s="9">
         <v>28.7</v>
       </c>
-      <c r="C7" s="10">
+      <c r="C7" s="9">
         <v>18.559999999999999</v>
       </c>
-      <c r="D7" s="10">
+      <c r="D7" s="9">
         <v>16.329999999999998</v>
       </c>
-      <c r="E7" s="10">
+      <c r="E7" s="9">
         <v>17.350000000000001</v>
       </c>
-      <c r="F7" s="11">
+      <c r="F7" s="10">
         <v>25895</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="17.25" thickBot="1">
-      <c r="A8" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="B8" s="10">
+      <c r="A8" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" s="9">
         <v>28.6</v>
       </c>
-      <c r="C8" s="10">
+      <c r="C8" s="9">
         <v>13.56</v>
       </c>
-      <c r="D8" s="10">
+      <c r="D8" s="9">
         <v>12.33</v>
       </c>
-      <c r="E8" s="10">
+      <c r="E8" s="9">
         <v>13.35</v>
       </c>
-      <c r="F8" s="11">
+      <c r="F8" s="10">
         <v>22895</v>
       </c>
     </row>

</xml_diff>